<commit_message>
Miscellaneous refactoring. Added start of interface hierarchy for type references.
</commit_message>
<xml_diff>
--- a/Katydid-KotlGen-JVM/doc/ModelClasses.xlsx
+++ b/Katydid-KotlGen-JVM/doc/ModelClasses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Nordberg\Documents\Workspace\KotlGen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Nordberg\Documents\Workspace\Katydid\Katydid-KotlGen-JVM\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ECF591-BCAD-45EC-8699-621273575B9A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F29D8E0-2D92-4E0D-8788-E25E00D1E244}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14610" xr2:uid="{6F083C0E-B77B-4AA0-A844-43789C25E8F3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="126">
   <si>
     <t>Type</t>
   </si>
@@ -386,6 +386,27 @@
   </si>
   <si>
     <t>package</t>
+  </si>
+  <si>
+    <t>KgTypeReference</t>
+  </si>
+  <si>
+    <t>KgUserType</t>
+  </si>
+  <si>
+    <t>KgNullableType</t>
+  </si>
+  <si>
+    <t>KgFunctionType</t>
+  </si>
+  <si>
+    <t>KgDynamicType</t>
+  </si>
+  <si>
+    <t>KgInferredType</t>
+  </si>
+  <si>
+    <t>KgParenthesizedType</t>
   </si>
 </sst>
 </file>
@@ -768,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5541CB-498D-4334-8D29-941291DA3443}">
-  <dimension ref="B2:AI69"/>
+  <dimension ref="B2:AI77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB63" sqref="AB63"/>
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,7 +3787,7 @@
         <v>3</v>
       </c>
       <c r="Q69" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="R69" s="4" t="s">
         <v>3</v>
@@ -3796,13 +3817,342 @@
         <v>3</v>
       </c>
       <c r="AA69" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AB69" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AC69" s="4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>119</v>
+      </c>
+      <c r="P71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA71" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC71" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>123</v>
+      </c>
+      <c r="P72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC72" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>122</v>
+      </c>
+      <c r="P73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC73" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>124</v>
+      </c>
+      <c r="P74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC74" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>121</v>
+      </c>
+      <c r="P75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC75" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>125</v>
+      </c>
+      <c r="P76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC76" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>120</v>
+      </c>
+      <c r="P77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC77" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised the way modifiers group and output. Started working on type parsing.
</commit_message>
<xml_diff>
--- a/Katydid-KotlGen-JVM/doc/ModelClasses.xlsx
+++ b/Katydid-KotlGen-JVM/doc/ModelClasses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Nordberg\Documents\Workspace\Katydid\Katydid-KotlGen-JVM\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F29D8E0-2D92-4E0D-8788-E25E00D1E244}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6612BCC7-DE33-43FA-A428-3E0DC478034B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14610" xr2:uid="{6F083C0E-B77B-4AA0-A844-43789C25E8F3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="127">
   <si>
     <t>Type</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>KgParenthesizedType</t>
+  </si>
+  <si>
+    <t>KgSimpleType</t>
   </si>
 </sst>
 </file>
@@ -789,10 +792,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5541CB-498D-4334-8D29-941291DA3443}">
-  <dimension ref="B2:AI77"/>
+  <dimension ref="B1:AI78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,60 +808,82 @@
     <col min="34" max="35" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:35" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AE2" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="2" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+    </row>
     <row r="3" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
@@ -877,9 +903,6 @@
       <c r="AG3" s="5"/>
     </row>
     <row r="4" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
@@ -894,213 +917,249 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
-      <c r="AE4" s="8"/>
+      <c r="AE4" s="5"/>
       <c r="AF4" s="5"/>
       <c r="AG4" s="5"/>
     </row>
-    <row r="5" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
+    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" t="s">
-        <v>72</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="U6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="V6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="W6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="X6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="C6" s="2"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
     </row>
     <row r="7" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="V8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="X8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC8" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
     </row>
     <row r="9" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
+      <c r="W9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI9" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
-        <v>4</v>
+      <c r="C10" s="2"/>
+      <c r="D10" t="s">
+        <v>20</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="W10" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="AB10" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="AC10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI10" s="3" t="s">
-        <v>33</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="4"/>
     </row>
     <row r="11" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
-      <c r="D11" t="s">
-        <v>20</v>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" t="s">
+        <v>55</v>
       </c>
       <c r="P11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="W11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>3</v>
+      <c r="X11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="Z11" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="AA11" s="4" t="s">
         <v>28</v>
@@ -1111,18 +1170,29 @@
       <c r="AC11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE11"/>
-      <c r="AF11"/>
-      <c r="AH11" s="4"/>
-      <c r="AI11" s="4"/>
+      <c r="AE11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI11" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P12" s="4" t="s">
         <v>28</v>
@@ -1185,10 +1255,10 @@
     <row r="13" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="O13" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="P13" s="4" t="s">
         <v>28</v>
@@ -1251,10 +1321,10 @@
     <row r="14" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>28</v>
@@ -1298,29 +1368,23 @@
       <c r="AC14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI14" s="4" t="s">
-        <v>8</v>
+      <c r="AG14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI14" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="O15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>28</v>
@@ -1364,23 +1428,29 @@
       <c r="AC15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI15" s="3" t="s">
-        <v>3</v>
+      <c r="AE15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI15" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:35" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O16" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="P16" s="4" t="s">
         <v>28</v>
@@ -1424,62 +1494,53 @@
       <c r="AC16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI16" s="5" t="s">
-        <v>8</v>
+      <c r="AG16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI16" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C17" s="2"/>
-      <c r="E17" t="s">
-        <v>58</v>
-      </c>
-      <c r="O17" t="s">
-        <v>52</v>
+      <c r="D17" t="s">
+        <v>24</v>
       </c>
       <c r="P17" s="4" t="s">
         <v>28</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="T17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="U17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="V17" s="5" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="W17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z17" s="5" t="s">
-        <v>28</v>
+      <c r="X17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="AA17" s="4" t="s">
         <v>28</v>
@@ -1490,53 +1551,52 @@
       <c r="AC17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI17" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="5"/>
     </row>
     <row r="18" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
-      <c r="D18" t="s">
-        <v>24</v>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="O18" t="s">
+        <v>38</v>
       </c>
       <c r="P18" s="4" t="s">
         <v>28</v>
       </c>
       <c r="Q18" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="S18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="U18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V18" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="V18" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="W18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z18" s="4" t="s">
-        <v>3</v>
+      <c r="X18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z18" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="AA18" s="4" t="s">
         <v>28</v>
@@ -1547,19 +1607,29 @@
       <c r="AC18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE18" s="5"/>
-      <c r="AF18" s="5"/>
-      <c r="AG18" s="5"/>
-      <c r="AH18" s="5"/>
-      <c r="AI18" s="5"/>
+      <c r="AE18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI18" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P19" s="4" t="s">
         <v>28</v>
@@ -1621,44 +1691,36 @@
     </row>
     <row r="20" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-      <c r="O20" t="s">
-        <v>39</v>
+      <c r="D20" t="s">
+        <v>5</v>
       </c>
       <c r="P20" s="4" t="s">
         <v>28</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="R20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="S20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="T20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="U20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="V20" s="5" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="S20" s="5"/>
+      <c r="T20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="W20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z20" s="6" t="s">
-        <v>28</v>
+      <c r="X20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y20" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="AA20" s="4" t="s">
         <v>28</v>
@@ -1669,54 +1731,51 @@
       <c r="AC20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI20" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AH20" s="4"/>
+      <c r="AI20" s="4"/>
     </row>
     <row r="21" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
-      <c r="D21" t="s">
-        <v>5</v>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" t="s">
+        <v>40</v>
       </c>
       <c r="P21" s="4" t="s">
         <v>28</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="S21" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="S21" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="T21" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="V21" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="W21" s="4" t="s">
         <v>28</v>
       </c>
       <c r="X21" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="Y21" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="AA21" s="4" t="s">
         <v>28</v>
@@ -1727,18 +1786,26 @@
       <c r="AC21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE21"/>
-      <c r="AF21"/>
-      <c r="AH21" s="4"/>
-      <c r="AI21" s="4"/>
+      <c r="AF21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI21" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P22" s="4" t="s">
         <v>28</v>
@@ -1782,7 +1849,10 @@
       <c r="AC22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF22" s="3" t="s">
+      <c r="AE22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AG22" s="4" t="s">
@@ -1792,16 +1862,16 @@
         <v>8</v>
       </c>
       <c r="AI22" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="O23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P23" s="4" t="s">
         <v>28</v>
@@ -1813,7 +1883,7 @@
         <v>28</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="T23" s="4" t="s">
         <v>28</v>
@@ -1834,7 +1904,7 @@
         <v>28</v>
       </c>
       <c r="Z23" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AA23" s="4" t="s">
         <v>28</v>
@@ -1845,29 +1915,23 @@
       <c r="AC23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI23" s="4" t="s">
-        <v>8</v>
+      <c r="AG23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI23" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="O24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P24" s="4" t="s">
         <v>28</v>
@@ -1879,7 +1943,7 @@
         <v>28</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="T24" s="4" t="s">
         <v>28</v>
@@ -1900,7 +1964,7 @@
         <v>28</v>
       </c>
       <c r="Z24" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AA24" s="4" t="s">
         <v>28</v>
@@ -1911,23 +1975,29 @@
       <c r="AC24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI24" s="3" t="s">
-        <v>3</v>
+      <c r="AE24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI24" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P25" s="4" t="s">
         <v>28</v>
@@ -1960,7 +2030,7 @@
         <v>28</v>
       </c>
       <c r="Z25" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AA25" s="4" t="s">
         <v>28</v>
@@ -1971,10 +2041,7 @@
       <c r="AC25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF25" s="4" t="s">
+      <c r="AF25" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AG25" s="4" t="s">
@@ -1984,16 +2051,16 @@
         <v>8</v>
       </c>
       <c r="AI25" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C26" s="2"/>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P26" s="4" t="s">
         <v>28</v>
@@ -2026,7 +2093,7 @@
         <v>28</v>
       </c>
       <c r="Z26" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AA26" s="4" t="s">
         <v>28</v>
@@ -2053,10 +2120,10 @@
     <row r="27" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P27" s="4" t="s">
         <v>28</v>
@@ -2089,7 +2156,7 @@
         <v>28</v>
       </c>
       <c r="Z27" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AA27" s="4" t="s">
         <v>28</v>
@@ -2115,41 +2182,41 @@
     </row>
     <row r="28" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C28" s="2"/>
-      <c r="E28" t="s">
-        <v>14</v>
+      <c r="D28" t="s">
+        <v>21</v>
       </c>
       <c r="O28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="U28" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="V28" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="W28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="X28" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="Z28" s="4" t="s">
         <v>3</v>
@@ -2163,35 +2230,32 @@
       <c r="AC28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI28" s="4" t="s">
+      <c r="AG28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI28" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="O29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P29" s="4" t="s">
         <v>28</v>
       </c>
       <c r="Q29" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="S29" s="5" t="s">
         <v>3</v>
@@ -2239,10 +2303,10 @@
     <row r="30" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="O30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P30" s="4" t="s">
         <v>28</v>
@@ -2254,7 +2318,7 @@
         <v>8</v>
       </c>
       <c r="S30" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="T30" s="4" t="s">
         <v>3</v>
@@ -2290,7 +2354,7 @@
         <v>3</v>
       </c>
       <c r="AH30" s="3" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="AI30" s="3" t="s">
         <v>3</v>
@@ -2299,10 +2363,10 @@
     <row r="31" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C31" s="2"/>
       <c r="D31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P31" s="4" t="s">
         <v>28</v>
@@ -2317,7 +2381,7 @@
         <v>8</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="U31" s="4" t="s">
         <v>3</v>
@@ -2335,7 +2399,7 @@
         <v>3</v>
       </c>
       <c r="Z31" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AA31" s="4" t="s">
         <v>28</v>
@@ -2347,10 +2411,10 @@
         <v>28</v>
       </c>
       <c r="AG31" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AH31" s="3" t="s">
-        <v>116</v>
+        <v>3</v>
       </c>
       <c r="AI31" s="3" t="s">
         <v>3</v>
@@ -2358,115 +2422,103 @@
     </row>
     <row r="32" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C32" s="2"/>
-      <c r="D32" t="s">
-        <v>29</v>
-      </c>
-      <c r="O32" t="s">
-        <v>50</v>
-      </c>
-      <c r="P32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="S32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="U32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI32" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
     </row>
     <row r="33" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C33" s="2"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
+      <c r="C33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB33" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="34" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C34" s="2" t="s">
-        <v>30</v>
+      <c r="C34" s="2"/>
+      <c r="D34" t="s">
+        <v>79</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="Q34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="S34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="T34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="U34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="V34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="W34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="X34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="Z34" s="4" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="AA34" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="AB34" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
+      </c>
+      <c r="AC34" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="P35" s="4" t="s">
         <v>28</v>
@@ -2514,7 +2566,10 @@
     <row r="36" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C36" s="2"/>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>105</v>
+      </c>
+      <c r="O36" t="s">
+        <v>102</v>
       </c>
       <c r="P36" s="4" t="s">
         <v>28</v>
@@ -2562,10 +2617,7 @@
     <row r="37" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C37" s="2"/>
       <c r="D37" t="s">
-        <v>105</v>
-      </c>
-      <c r="O37" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="P37" s="4" t="s">
         <v>28</v>
@@ -2612,8 +2664,11 @@
     </row>
     <row r="38" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
-      <c r="D38" t="s">
-        <v>80</v>
+      <c r="E38" t="s">
+        <v>73</v>
+      </c>
+      <c r="O38" t="s">
+        <v>89</v>
       </c>
       <c r="P38" s="4" t="s">
         <v>28</v>
@@ -2649,22 +2704,22 @@
         <v>28</v>
       </c>
       <c r="AA38" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="AB38" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AC38" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="O39" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P39" s="4" t="s">
         <v>28</v>
@@ -2712,10 +2767,10 @@
     <row r="40" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
       <c r="E40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P40" s="4" t="s">
         <v>28</v>
@@ -2763,10 +2818,10 @@
     <row r="41" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="E41" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O41" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P41" s="4" t="s">
         <v>28</v>
@@ -2808,16 +2863,13 @@
         <v>28</v>
       </c>
       <c r="AC41" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C42" s="2"/>
-      <c r="E42" t="s">
-        <v>83</v>
-      </c>
-      <c r="O42" t="s">
-        <v>92</v>
+      <c r="D42" t="s">
+        <v>75</v>
       </c>
       <c r="P42" s="4" t="s">
         <v>28</v>
@@ -2850,9 +2902,6 @@
         <v>28</v>
       </c>
       <c r="Z42" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA42" s="4" t="s">
         <v>28</v>
       </c>
       <c r="AB42" s="4" t="s">
@@ -2864,59 +2913,65 @@
     </row>
     <row r="43" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
-      <c r="D43" t="s">
-        <v>75</v>
-      </c>
-      <c r="P43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB43" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC43" s="4" t="s">
-        <v>3</v>
+      <c r="E43" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
-      <c r="E44" t="s">
-        <v>108</v>
+      <c r="D44" t="s">
+        <v>84</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA44" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC44" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
-      <c r="D45" t="s">
-        <v>84</v>
+      <c r="E45" t="s">
+        <v>86</v>
+      </c>
+      <c r="O45" t="s">
+        <v>93</v>
       </c>
       <c r="P45" s="4" t="s">
         <v>28</v>
@@ -2952,7 +3007,7 @@
         <v>28</v>
       </c>
       <c r="AA45" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="AB45" s="4" t="s">
         <v>28</v>
@@ -2964,10 +3019,10 @@
     <row r="46" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C46" s="2"/>
       <c r="E46" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P46" s="4" t="s">
         <v>28</v>
@@ -3015,10 +3070,10 @@
     <row r="47" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C47" s="2"/>
       <c r="E47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O47" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P47" s="4" t="s">
         <v>28</v>
@@ -3065,11 +3120,8 @@
     </row>
     <row r="48" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C48" s="2"/>
-      <c r="E48" t="s">
-        <v>85</v>
-      </c>
-      <c r="O48" t="s">
-        <v>95</v>
+      <c r="D48" t="s">
+        <v>31</v>
       </c>
       <c r="P48" s="4" t="s">
         <v>28</v>
@@ -3105,7 +3157,7 @@
         <v>28</v>
       </c>
       <c r="AA48" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="AB48" s="4" t="s">
         <v>28</v>
@@ -3117,7 +3169,7 @@
     <row r="49" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C49" s="2"/>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="P49" s="4" t="s">
         <v>28</v>
@@ -3153,7 +3205,7 @@
         <v>28</v>
       </c>
       <c r="AA49" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AB49" s="4" t="s">
         <v>28</v>
@@ -3165,7 +3217,7 @@
     <row r="50" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C50" s="2"/>
       <c r="D50" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P50" s="4" t="s">
         <v>28</v>
@@ -3213,7 +3265,10 @@
     <row r="51" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C51" s="2"/>
       <c r="D51" t="s">
-        <v>74</v>
+        <v>103</v>
+      </c>
+      <c r="O51" t="s">
+        <v>96</v>
       </c>
       <c r="P51" s="4" t="s">
         <v>28</v>
@@ -3255,16 +3310,16 @@
         <v>28</v>
       </c>
       <c r="AC51" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C52" s="2"/>
       <c r="D52" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O52" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P52" s="4" t="s">
         <v>28</v>
@@ -3312,10 +3367,10 @@
     <row r="53" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C53" s="2"/>
       <c r="D53" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="O53" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P53" s="4" t="s">
         <v>28</v>
@@ -3357,16 +3412,16 @@
         <v>28</v>
       </c>
       <c r="AC53" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C54" s="2"/>
       <c r="D54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O54" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P54" s="4" t="s">
         <v>28</v>
@@ -3413,516 +3468,465 @@
     </row>
     <row r="55" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C55" s="2"/>
-      <c r="D55" t="s">
-        <v>107</v>
-      </c>
-      <c r="O55" t="s">
-        <v>99</v>
-      </c>
-      <c r="P55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA55" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC55" s="4" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="56" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C56" s="2"/>
+      <c r="D56" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="57" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C57" s="2"/>
-      <c r="D57" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="58" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C58" s="2"/>
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="O58" t="s">
+        <v>110</v>
+      </c>
+      <c r="P58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="T58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="U58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y58" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC58" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>1</v>
-      </c>
-      <c r="O59" t="s">
-        <v>110</v>
-      </c>
-      <c r="P59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q59" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="R59" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="S59" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T59" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="U59" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="V59" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="W59" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="X59" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y59" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB59" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC59" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+      <c r="T59" s="5"/>
+      <c r="U59" s="5"/>
+      <c r="V59" s="5"/>
+      <c r="W59" s="5"/>
+      <c r="X59" s="5"/>
+      <c r="Y59" s="5"/>
     </row>
     <row r="60" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="Q60" s="5"/>
-      <c r="R60" s="5"/>
-      <c r="S60" s="5"/>
-      <c r="T60" s="5"/>
-      <c r="U60" s="5"/>
-      <c r="V60" s="5"/>
-      <c r="W60" s="5"/>
-      <c r="X60" s="5"/>
-      <c r="Y60" s="5"/>
-    </row>
-    <row r="61" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+      <c r="C60" t="s">
         <v>117</v>
       </c>
-      <c r="O61" t="s">
+      <c r="O60" t="s">
         <v>118</v>
       </c>
-      <c r="P61" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="R61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="S61" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="U61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="V61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="W61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="X61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC61" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
+      <c r="P60" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="U60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="V60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="X60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC60" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>126</v>
+      </c>
+      <c r="P62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC62" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
         <v>6</v>
       </c>
-      <c r="P63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q63" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R63" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="S63" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T63" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="V63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="W63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="X63" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y63" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z63" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC63" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+      <c r="P64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="R64" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="S64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T64" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="W64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X64" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y64" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z64" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC64" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
         <v>68</v>
       </c>
-      <c r="P65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="R65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="X65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC65" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D66" t="s">
-        <v>69</v>
-      </c>
-      <c r="O66" t="s">
-        <v>100</v>
-      </c>
       <c r="P66" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="Q66" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="R66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="S66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="T66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="U66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="V66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="W66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="X66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="Y66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="Z66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="AA66" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="AB66" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="AC66" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
+        <v>69</v>
+      </c>
+      <c r="O67" t="s">
+        <v>100</v>
+      </c>
+      <c r="P67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB67" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC67" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
         <v>70</v>
       </c>
-      <c r="O67" t="s">
+      <c r="O68" t="s">
         <v>101</v>
       </c>
-      <c r="P67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB67" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC67" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
+      <c r="P68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC68" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
         <v>115</v>
       </c>
-      <c r="P69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q69" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="R69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="X69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z69" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA69" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB69" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC69" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
+      <c r="P70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z70" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC70" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>119</v>
       </c>
-      <c r="P71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="V71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="X71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA71" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC71" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
-        <v>123</v>
-      </c>
       <c r="P72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="Q72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="R72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="S72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="T72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="U72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="V72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="W72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="X72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="Y72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="Z72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="AA72" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="AB72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="AC72" s="4" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P73" s="4" t="s">
         <v>28</v>
@@ -3969,7 +3973,7 @@
     </row>
     <row r="74" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P74" s="4" t="s">
         <v>28</v>
@@ -4016,7 +4020,7 @@
     </row>
     <row r="75" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="P75" s="4" t="s">
         <v>28</v>
@@ -4063,7 +4067,7 @@
     </row>
     <row r="76" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="P76" s="4" t="s">
         <v>28</v>
@@ -4110,48 +4114,95 @@
     </row>
     <row r="77" spans="3:29" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
+        <v>125</v>
+      </c>
+      <c r="P77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC77" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
         <v>120</v>
       </c>
-      <c r="P77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC77" s="4" t="s">
+      <c r="P78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="V78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC78" s="4" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Work in progress for representing types. Added documentation to a few core classes.
</commit_message>
<xml_diff>
--- a/Katydid-KotlGen-JVM/doc/ModelClasses.xlsx
+++ b/Katydid-KotlGen-JVM/doc/ModelClasses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Nordberg\Documents\Workspace\Katydid\Katydid-KotlGen-JVM\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6612BCC7-DE33-43FA-A428-3E0DC478034B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2617A1AE-8A03-4C41-B3F6-BDCA63085537}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14610" xr2:uid="{6F083C0E-B77B-4AA0-A844-43789C25E8F3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="121">
   <si>
     <t>Type</t>
   </si>
@@ -389,24 +389,6 @@
   </si>
   <si>
     <t>KgTypeReference</t>
-  </si>
-  <si>
-    <t>KgUserType</t>
-  </si>
-  <si>
-    <t>KgNullableType</t>
-  </si>
-  <si>
-    <t>KgFunctionType</t>
-  </si>
-  <si>
-    <t>KgDynamicType</t>
-  </si>
-  <si>
-    <t>KgInferredType</t>
-  </si>
-  <si>
-    <t>KgParenthesizedType</t>
   </si>
   <si>
     <t>KgSimpleType</t>
@@ -792,11 +774,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5541CB-498D-4334-8D29-941291DA3443}">
-  <dimension ref="B1:AI78"/>
+  <dimension ref="B1:AI72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,7 +3573,7 @@
     </row>
     <row r="62" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="P62" s="4" t="s">
         <v>3</v>
@@ -3922,288 +3904,6 @@
       </c>
       <c r="AC72" s="4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
-        <v>123</v>
-      </c>
-      <c r="P73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB73" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC73" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="74" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>122</v>
-      </c>
-      <c r="P74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB74" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC74" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="75" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>124</v>
-      </c>
-      <c r="P75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC75" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>121</v>
-      </c>
-      <c r="P76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB76" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC76" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>125</v>
-      </c>
-      <c r="P77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC77" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="78" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D78" t="s">
-        <v>120</v>
-      </c>
-      <c r="P78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="R78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB78" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC78" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on type parsing.
</commit_message>
<xml_diff>
--- a/Katydid-KotlGen-JVM/doc/ModelClasses.xlsx
+++ b/Katydid-KotlGen-JVM/doc/ModelClasses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Nordberg\Documents\Workspace\Katydid\Katydid-KotlGen-JVM\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2617A1AE-8A03-4C41-B3F6-BDCA63085537}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A7113F-714E-4C85-AAEA-5300AC8B2DEB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14610" xr2:uid="{6F083C0E-B77B-4AA0-A844-43789C25E8F3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="122">
   <si>
     <t>Type</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t>KgSimpleType</t>
+  </si>
+  <si>
+    <t>Parameterized?</t>
   </si>
 </sst>
 </file>
@@ -774,23 +777,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5541CB-498D-4334-8D29-941291DA3443}">
-  <dimension ref="B1:AI72"/>
+  <dimension ref="B1:AJ72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K75" sqref="K75"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD70" sqref="AD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="14" width="3.85546875" customWidth="1"/>
     <col min="15" max="15" width="21" customWidth="1"/>
-    <col min="16" max="29" width="13.7109375" style="4" customWidth="1"/>
-    <col min="31" max="33" width="11.28515625" style="4" customWidth="1"/>
-    <col min="34" max="35" width="11.28515625" customWidth="1"/>
+    <col min="16" max="30" width="13.7109375" style="4" customWidth="1"/>
+    <col min="32" max="34" width="11.28515625" style="4" customWidth="1"/>
+    <col min="35" max="36" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:36" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,11 +842,14 @@
       <c r="AC1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AD1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF1" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
@@ -858,11 +864,12 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AF2" s="8"/>
       <c r="AG2" s="5"/>
-    </row>
-    <row r="3" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH2" s="5"/>
+    </row>
+    <row r="3" spans="2:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>109</v>
       </c>
@@ -880,11 +887,12 @@
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AF3" s="8"/>
       <c r="AG3" s="5"/>
-    </row>
-    <row r="4" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH3" s="5"/>
+    </row>
+    <row r="4" spans="2:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
@@ -899,11 +907,12 @@
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
-      <c r="AE4" s="5"/>
+      <c r="AD4" s="5"/>
       <c r="AF4" s="5"/>
       <c r="AG4" s="5"/>
-    </row>
-    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AH4" s="5"/>
+    </row>
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -953,13 +962,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
     </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -1006,13 +1015,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
     </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
@@ -1034,23 +1043,23 @@
       <c r="AC9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AE9" s="3" t="s">
+      <c r="AF9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AF9" s="3" t="s">
+      <c r="AG9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AG9" s="3" t="s">
+      <c r="AH9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AH9" s="3" t="s">
+      <c r="AI9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AI9" s="3" t="s">
+      <c r="AJ9" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" t="s">
         <v>20</v>
@@ -1097,12 +1106,15 @@
       <c r="AC10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE10"/>
+      <c r="AD10" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="AF10"/>
-      <c r="AH10" s="4"/>
+      <c r="AG10"/>
       <c r="AI10" s="4"/>
-    </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ10" s="4"/>
+    </row>
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="E11" t="s">
         <v>22</v>
@@ -1152,10 +1164,10 @@
       <c r="AC11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF11" s="4" t="s">
+      <c r="AD11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AG11" s="4" t="s">
@@ -1167,8 +1179,11 @@
       <c r="AI11" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="E12" t="s">
         <v>23</v>
@@ -1218,10 +1233,10 @@
       <c r="AC12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF12" s="4" t="s">
+      <c r="AD12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AG12" s="4" t="s">
@@ -1233,8 +1248,11 @@
       <c r="AI12" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="E13" t="s">
         <v>37</v>
@@ -1284,10 +1302,10 @@
       <c r="AC13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF13" s="4" t="s">
+      <c r="AD13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AG13" s="4" t="s">
@@ -1299,8 +1317,11 @@
       <c r="AI13" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="E14" t="s">
         <v>36</v>
@@ -1350,17 +1371,20 @@
       <c r="AC14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG14" s="3" t="s">
-        <v>3</v>
+      <c r="AD14" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="AH14" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AI14" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="E15" t="s">
         <v>57</v>
@@ -1410,13 +1434,13 @@
       <c r="AC15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG15" s="5" t="s">
+      <c r="AD15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AH15" s="5" t="s">
@@ -1425,8 +1449,11 @@
       <c r="AI15" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="AJ15" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="E16" t="s">
         <v>58</v>
@@ -1476,17 +1503,20 @@
       <c r="AC16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG16" s="3" t="s">
-        <v>3</v>
+      <c r="AD16" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="AH16" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AI16" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="3:35" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="AJ16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C17" s="2"/>
       <c r="D17" t="s">
         <v>24</v>
@@ -1533,13 +1563,16 @@
       <c r="AC17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE17" s="5"/>
+      <c r="AD17" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="AF17" s="5"/>
       <c r="AG17" s="5"/>
       <c r="AH17" s="5"/>
       <c r="AI17" s="5"/>
-    </row>
-    <row r="18" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="AJ17" s="5"/>
+    </row>
+    <row r="18" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
       <c r="E18" t="s">
         <v>25</v>
@@ -1589,10 +1622,10 @@
       <c r="AC18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF18" s="5" t="s">
+      <c r="AD18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AG18" s="5" t="s">
@@ -1604,8 +1637,11 @@
       <c r="AI18" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="AJ18" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="E19" t="s">
         <v>26</v>
@@ -1655,10 +1691,10 @@
       <c r="AC19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF19" s="5" t="s">
+      <c r="AD19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AG19" s="5" t="s">
@@ -1670,8 +1706,11 @@
       <c r="AI19" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="AJ19" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" t="s">
         <v>5</v>
@@ -1713,12 +1752,15 @@
       <c r="AC20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE20"/>
+      <c r="AD20" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="AF20"/>
-      <c r="AH20" s="4"/>
+      <c r="AG20"/>
       <c r="AI20" s="4"/>
-    </row>
-    <row r="21" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="AJ20" s="4"/>
+    </row>
+    <row r="21" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="E21" t="s">
         <v>9</v>
@@ -1768,20 +1810,23 @@
       <c r="AC21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG21" s="4" t="s">
+      <c r="AD21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AH21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AI21" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="3:35" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="AJ21" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="E22" t="s">
         <v>10</v>
@@ -1831,10 +1876,10 @@
       <c r="AC22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF22" s="4" t="s">
+      <c r="AD22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AG22" s="4" t="s">
@@ -1846,8 +1891,11 @@
       <c r="AI22" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="AJ22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="E23" t="s">
         <v>15</v>
@@ -1897,17 +1945,20 @@
       <c r="AC23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG23" s="3" t="s">
-        <v>3</v>
+      <c r="AD23" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="AH23" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AI23" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="3:35" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="AJ23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="E24" t="s">
         <v>11</v>
@@ -1957,10 +2008,10 @@
       <c r="AC24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AE24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF24" s="4" t="s">
+      <c r="AD24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AG24" s="4" t="s">
@@ -1972,8 +2023,11 @@
       <c r="AI24" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="AJ24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="E25" t="s">
         <v>12</v>
@@ -2023,20 +2077,23 @@
       <c r="AC25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG25" s="4" t="s">
+      <c r="AD25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG25" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AH25" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AI25" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="3:35" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="AJ25" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C26" s="2"/>
       <c r="E26" t="s">
         <v>13</v>
@@ -2086,20 +2143,23 @@
       <c r="AC26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG26" s="4" t="s">
+      <c r="AD26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AH26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AI26" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="3:35" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="AJ26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
       <c r="E27" t="s">
         <v>14</v>
@@ -2149,20 +2209,23 @@
       <c r="AC27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG27" s="4" t="s">
+      <c r="AD27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="AH27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AI27" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="3:35" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="AJ27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C28" s="2"/>
       <c r="D28" t="s">
         <v>21</v>
@@ -2212,17 +2275,20 @@
       <c r="AC28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG28" s="3" t="s">
+      <c r="AD28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="AH28" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AI28" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="3:35" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="AJ28" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" t="s">
         <v>67</v>
@@ -2272,17 +2338,20 @@
       <c r="AC29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG29" s="3" t="s">
-        <v>3</v>
+      <c r="AD29" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="AH29" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AI29" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="3:35" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="AJ29" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" t="s">
         <v>27</v>
@@ -2332,17 +2401,20 @@
       <c r="AC30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG30" s="3" t="s">
+      <c r="AD30" s="4" t="s">
         <v>3</v>
       </c>
       <c r="AH30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI30" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="AI30" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="AJ30" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C31" s="2"/>
       <c r="D31" t="s">
         <v>29</v>
@@ -2392,23 +2464,26 @@
       <c r="AC31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AG31" s="3" t="s">
-        <v>8</v>
+      <c r="AD31" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="AH31" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AI31" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="AJ31" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C32" s="2"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
     </row>
-    <row r="33" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C33" s="2" t="s">
         <v>30</v>
       </c>
@@ -2448,8 +2523,11 @@
       <c r="AB33" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD33" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C34" s="2"/>
       <c r="D34" t="s">
         <v>79</v>
@@ -2496,8 +2574,11 @@
       <c r="AC34" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD34" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>
       <c r="D35" t="s">
         <v>76</v>
@@ -2544,8 +2625,11 @@
       <c r="AC35" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD35" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C36" s="2"/>
       <c r="D36" t="s">
         <v>105</v>
@@ -2595,8 +2679,11 @@
       <c r="AC36" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD36" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C37" s="2"/>
       <c r="D37" t="s">
         <v>80</v>
@@ -2643,8 +2730,11 @@
       <c r="AC37" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD37" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
       <c r="E38" t="s">
         <v>73</v>
@@ -2694,8 +2784,11 @@
       <c r="AC38" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD38" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="E39" t="s">
         <v>81</v>
@@ -2745,8 +2838,11 @@
       <c r="AC39" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD39" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
       <c r="E40" t="s">
         <v>82</v>
@@ -2796,8 +2892,11 @@
       <c r="AC40" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD40" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="E41" t="s">
         <v>83</v>
@@ -2847,8 +2946,11 @@
       <c r="AC41" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD41" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C42" s="2"/>
       <c r="D42" t="s">
         <v>75</v>
@@ -2892,14 +2994,20 @@
       <c r="AC42" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD42" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
       <c r="E43" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="44" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD43" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
       <c r="D44" t="s">
         <v>84</v>
@@ -2946,8 +3054,11 @@
       <c r="AC44" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD44" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
       <c r="E45" t="s">
         <v>86</v>
@@ -2997,8 +3108,11 @@
       <c r="AC45" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD45" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C46" s="2"/>
       <c r="E46" t="s">
         <v>87</v>
@@ -3048,8 +3162,11 @@
       <c r="AC46" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD46" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C47" s="2"/>
       <c r="E47" t="s">
         <v>85</v>
@@ -3099,8 +3216,11 @@
       <c r="AC47" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD47" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C48" s="2"/>
       <c r="D48" t="s">
         <v>31</v>
@@ -3147,8 +3267,11 @@
       <c r="AC48" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD48" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C49" s="2"/>
       <c r="D49" t="s">
         <v>78</v>
@@ -3195,8 +3318,11 @@
       <c r="AC49" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD49" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C50" s="2"/>
       <c r="D50" t="s">
         <v>74</v>
@@ -3243,8 +3369,11 @@
       <c r="AC50" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD50" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C51" s="2"/>
       <c r="D51" t="s">
         <v>103</v>
@@ -3294,8 +3423,11 @@
       <c r="AC51" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD51" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C52" s="2"/>
       <c r="D52" t="s">
         <v>104</v>
@@ -3345,8 +3477,11 @@
       <c r="AC52" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD52" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C53" s="2"/>
       <c r="D53" t="s">
         <v>106</v>
@@ -3396,8 +3531,11 @@
       <c r="AC53" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD53" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C54" s="2"/>
       <c r="D54" t="s">
         <v>107</v>
@@ -3447,20 +3585,23 @@
       <c r="AC54" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD54" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C56" s="2"/>
       <c r="D56" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>1</v>
       </c>
@@ -3509,8 +3650,11 @@
       <c r="AC58" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD58" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="3:30" x14ac:dyDescent="0.25">
       <c r="Q59" s="5"/>
       <c r="R59" s="5"/>
       <c r="S59" s="5"/>
@@ -3521,7 +3665,7 @@
       <c r="X59" s="5"/>
       <c r="Y59" s="5"/>
     </row>
-    <row r="60" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>117</v>
       </c>
@@ -3570,8 +3714,11 @@
       <c r="AC60" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD60" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>120</v>
       </c>
@@ -3617,8 +3764,11 @@
       <c r="AC62" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD62" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>6</v>
       </c>
@@ -3664,8 +3814,11 @@
       <c r="AC64" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD64" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>68</v>
       </c>
@@ -3711,8 +3864,11 @@
       <c r="AC66" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD66" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>69</v>
       </c>
@@ -3761,8 +3917,11 @@
       <c r="AC67" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="68" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD67" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>70</v>
       </c>
@@ -3811,8 +3970,11 @@
       <c r="AC68" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="70" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD68" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>115</v>
       </c>
@@ -3858,8 +4020,11 @@
       <c r="AC70" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AD70" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>119</v>
       </c>
@@ -3903,6 +4068,9 @@
         <v>3</v>
       </c>
       <c r="AC72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD72" s="4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>